<commit_message>
Atualização do arquivo abastecimento.xlsx
</commit_message>
<xml_diff>
--- a/datasets/abastecimento.xlsx
+++ b/datasets/abastecimento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FranklinAlves\.devFk\.eu_dev\automation_selenium\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1782B7-9EFA-4486-A11D-DC682A259D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34369ABD-2595-41CD-98C3-3C4C76F633F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6060" yWindow="3705" windowWidth="17040" windowHeight="10710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>DATA</t>
   </si>
@@ -79,12 +79,6 @@
   </si>
   <si>
     <t>1430</t>
-  </si>
-  <si>
-    <t>0700</t>
-  </si>
-  <si>
-    <t>1120</t>
   </si>
   <si>
     <t xml:space="preserve">Gasolina </t>
@@ -467,7 +461,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,22 +491,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>45509</v>
+        <v>45536</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="6">
-        <v>41.25</v>
+        <v>43.250999999999998</v>
       </c>
       <c r="E2" s="7">
-        <v>95214</v>
+        <v>96349.259000000005</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>9</v>
@@ -520,7 +514,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>45517</v>
+        <v>45537</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -530,10 +524,10 @@
         <v>PLC-0001</v>
       </c>
       <c r="D3" s="6">
-        <v>42.057000000000002</v>
+        <v>45.222000000000001</v>
       </c>
       <c r="E3" s="7">
-        <v>95550.456000000006</v>
+        <v>96756.257000000012</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>8</v>
@@ -544,7 +538,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>45523</v>
+        <v>45538</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -554,10 +548,10 @@
         <v>PLC-0001</v>
       </c>
       <c r="D4" s="6">
-        <v>39.54</v>
+        <v>47.253</v>
       </c>
       <c r="E4" s="7">
-        <v>95866.776000000013</v>
+        <v>97181.534000000014</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>8</v>
@@ -568,7 +562,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>45526</v>
+        <v>45539</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
@@ -578,10 +572,10 @@
         <v>PLC-0001</v>
       </c>
       <c r="D5" s="6">
-        <v>37.020000000000003</v>
+        <v>44.529000000000003</v>
       </c>
       <c r="E5" s="7">
-        <v>96162.936000000016</v>
+        <v>97582.295000000013</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>8</v>
@@ -592,7 +586,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>45532</v>
+        <v>45540</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
@@ -602,10 +596,10 @@
         <v>PLC-0001</v>
       </c>
       <c r="D6" s="6">
-        <v>42.65</v>
+        <v>42.369</v>
       </c>
       <c r="E6" s="7">
-        <v>96504.136000000013</v>
+        <v>97963.616000000009</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>8</v>
@@ -616,19 +610,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>45506</v>
+        <v>45541</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="6">
-        <v>43.25</v>
+        <v>41.253999999999998</v>
       </c>
       <c r="E7" s="7">
-        <v>93119.25</v>
+        <v>96830.032000000007</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>8</v>
@@ -639,7 +633,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>45511</v>
+        <v>45542</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -649,10 +643,10 @@
         <v>PLC-0002</v>
       </c>
       <c r="D8" s="6">
-        <v>45</v>
+        <v>42.057000000000002</v>
       </c>
       <c r="E8" s="7">
-        <v>93524.25</v>
+        <v>97166.488000000012</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>8</v>
@@ -663,7 +657,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>45513</v>
+        <v>45543</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>11</v>
@@ -673,10 +667,10 @@
         <v>PLC-0002</v>
       </c>
       <c r="D9" s="6">
-        <v>47.25</v>
+        <v>39.546999999999997</v>
       </c>
       <c r="E9" s="7">
-        <v>93949.5</v>
+        <v>97482.864000000016</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>8</v>
@@ -687,7 +681,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>45517</v>
+        <v>45544</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>13</v>
@@ -697,10 +691,10 @@
         <v>PLC-0002</v>
       </c>
       <c r="D10" s="6">
-        <v>44.52</v>
+        <v>37.027000000000001</v>
       </c>
       <c r="E10" s="7">
-        <v>94350.18</v>
+        <v>97779.080000000016</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>8</v>
@@ -711,7 +705,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>45520</v>
+        <v>45545</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>14</v>
@@ -721,10 +715,10 @@
         <v>PLC-0002</v>
       </c>
       <c r="D11" s="6">
-        <v>42.369</v>
+        <v>42.658000000000001</v>
       </c>
       <c r="E11" s="7">
-        <v>94731.500999999989</v>
+        <v>98120.344000000012</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>8</v>
@@ -734,76 +728,31 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>45524</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>PLC-0002</v>
-      </c>
-      <c r="D12" s="6">
-        <v>43.25</v>
-      </c>
-      <c r="E12" s="7">
-        <v>95120.750999999989</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>45527</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>PLC-0002</v>
-      </c>
-      <c r="D13" s="6">
-        <v>46.99</v>
-      </c>
-      <c r="E13" s="7">
-        <v>95543.660999999993</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>45533</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>PLC-0002</v>
-      </c>
-      <c r="D14" s="6">
-        <v>46.320999999999998</v>
-      </c>
-      <c r="E14" s="7">
-        <v>95960.549999999988</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" s="8"/>
@@ -816,7 +765,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:B14 G2:G14" numberStoredAsText="1"/>
+    <ignoredError sqref="B2:B11 G2:G11" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>